<commit_message>
removed the print statements from catch block
</commit_message>
<xml_diff>
--- a/Maven_Automation/Result/DWWorkspace/WorkspaceCreation/DWWorkspace_WorkspaceCreation.xlsx
+++ b/Maven_Automation/Result/DWWorkspace/WorkspaceCreation/DWWorkspace_WorkspaceCreation.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>TestcaseID</t>
   </si>
@@ -86,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -126,6 +126,23 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
made changes to framework
</commit_message>
<xml_diff>
--- a/Maven_Automation/Result/DWWorkspace/WorkspaceCreation/DWWorkspace_WorkspaceCreation.xlsx
+++ b/Maven_Automation/Result/DWWorkspace/WorkspaceCreation/DWWorkspace_WorkspaceCreation.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
   <si>
     <t>TestcaseID</t>
   </si>
@@ -42,6 +42,25 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>TEAM Workspace Should be created successfully</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"id","selector":"menuTrigger"}
+  (Session info: chrome=56.0.2924.87)
+  (Driver info: chromedriver=2.25.426923 (0390b88869384d6eb0d5d09729679f934aab9eed),platform=Windows NT 10.0.14393 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 10.30 seconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.0.1', revision: '1969d75', time: '2016-10-18 09:49:13 -0700'
+System info: host: 'MQCSERVER', ip: '172.16.0.7', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_121'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.25.426923 (0390b88869384d6eb0d5d09729679f934aab9eed), userDataDir=C:\Users\admin\AppData\Local\Temp\scoped_dir4684_19381}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=56.0.2924.87, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
+Session ID: c0b590a1ff96b6bcb3d2cb09d870ccc7
+*** Element info: {Using=id, value=menuTrigger}</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -86,7 +105,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -143,6 +162,74 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
modified the test data path in driver.xlsx file and global methods.java file.
</commit_message>
<xml_diff>
--- a/Maven_Automation/Result/DWWorkspace/WorkspaceCreation/DWWorkspace_WorkspaceCreation.xlsx
+++ b/Maven_Automation/Result/DWWorkspace/WorkspaceCreation/DWWorkspace_WorkspaceCreation.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
   <si>
     <t>TestcaseID</t>
   </si>
@@ -105,7 +105,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -230,6 +230,23 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Added NewsArticle_Creation.java class and made changes in dirver and Reusable_Action.java classes
</commit_message>
<xml_diff>
--- a/Maven_Automation/Result/DWWorkspace/WorkspaceCreation/DWWorkspace_WorkspaceCreation.xlsx
+++ b/Maven_Automation/Result/DWWorkspace/WorkspaceCreation/DWWorkspace_WorkspaceCreation.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="14">
   <si>
     <t>TestcaseID</t>
   </si>
@@ -61,6 +61,19 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":".//*[@id='wsGrid3']/div[1]/div[1]/div[2]/div/div[1]/div/div[8]/div/a/span"}
+  (Session info: chrome=56.0.2924.87)
+  (Driver info: chromedriver=2.25.426923 (0390b88869384d6eb0d5d09729679f934aab9eed),platform=Windows NT 10.0.14393 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 10.35 seconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.0.1', revision: '1969d75', time: '2016-10-18 09:49:13 -0700'
+System info: host: 'MQCSERVER', ip: '172.16.0.6', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_121'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.25.426923 (0390b88869384d6eb0d5d09729679f934aab9eed), userDataDir=C:\Users\admin\AppData\Local\Temp\scoped_dir4028_26424}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=56.0.2924.87, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=true, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true}]
+Session ID: 95b176ce5c6d8567fb219bf37ddbfd7f
+*** Element info: {Using=xpath, value=.//*[@id='wsGrid3']/div[1]/div[1]/div[2]/div/div[1]/div/div[8]/div/a/span}</t>
   </si>
 </sst>
 </file>
@@ -105,7 +118,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -247,6 +260,57 @@
         <v>9</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>